<commit_message>
fix: ajustar para preencher dados a partir da linha 2 (A2) mantendo cabeçalho na linha 1
</commit_message>
<xml_diff>
--- a/Copy of Template - Cadastro Cliente(1).xlsx
+++ b/Copy of Template - Cadastro Cliente(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bel\Documents\CRM_Ymbale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bel\Documents\CRM_Ymbale\crm-ymbale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7625A897-914A-4303-889B-DAEB86CEB3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5BC9E3-922B-4845-92FF-A02771E20030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,7 +886,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nome</t>
   </si>
@@ -930,76 +930,7 @@
     <t>Clientes</t>
   </si>
   <si>
-    <t>Contato 1</t>
-  </si>
-  <si>
-    <t>joao@email.com.br</t>
-  </si>
-  <si>
-    <t>+55 27 98804-0460</t>
-  </si>
-  <si>
-    <t>+55 33 97682-9412</t>
-  </si>
-  <si>
-    <t>Rua do contato</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Sobrado nº3</t>
-  </si>
-  <si>
-    <t>Bairro 1</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>Paraná</t>
-  </si>
-  <si>
-    <t>Curitiba</t>
-  </si>
-  <si>
-    <t>48.858080, 2.294795</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>Contato 2</t>
-  </si>
-  <si>
-    <t>maria@email.com.br</t>
-  </si>
-  <si>
-    <t>+55 43 96884-4667</t>
-  </si>
-  <si>
-    <t>+55 21 98331-7664</t>
-  </si>
-  <si>
-    <t>Sobrado nº4</t>
-  </si>
-  <si>
-    <t>Bairro 2</t>
-  </si>
-  <si>
-    <t>48.858080, 2.294796</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
     <t>E-mail</t>
-  </si>
-  <si>
-    <t>Cliente 1</t>
-  </si>
-  <si>
-    <t>Cliente 1;Cliente 2</t>
   </si>
   <si>
     <t>Código Cliente</t>
@@ -1484,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1551,105 +1482,31 @@
         <v>12</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2">
-        <v>8888888</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3">
-        <v>8888888</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1764,13 +1621,9 @@
       <c r="F17" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1699632147" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">

</xml_diff>